<commit_message>
String to int[] 함수 추가
</commit_message>
<xml_diff>
--- a/Project-S/Assets/Excel/ExcelFile/TimeTable.xlsx
+++ b/Project-S/Assets/Excel/ExcelFile/TimeTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fork\Project-S\Project-S\Assets\Excel\ExcelFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\Project-S\Project-S\Assets\Excel\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4286B92-A7BB-42CB-8B35-B04E7B9A99B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7152260-A402-4736-A0CC-84A66BBB1A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2EA46A0F-1C0F-40B9-A7DB-A9EB9D9B0369}"/>
+    <workbookView xWindow="5895" yWindow="2640" windowWidth="21645" windowHeight="11835" xr2:uid="{2EA46A0F-1C0F-40B9-A7DB-A9EB9D9B0369}"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="1" r:id="rId1"/>
@@ -47,14 +47,15 @@
     <t>maxDay</t>
   </si>
   <si>
-    <t>[0,1,2,3,4,5]</t>
-  </si>
-  <si>
     <t>weatherType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[0,1,2,3,4,5]</t>
+    <t>0;1;2;3;4;5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;1;2;3;4;5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -422,7 +423,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -445,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -459,7 +460,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -473,7 +474,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -487,7 +488,7 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -501,7 +502,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>